<commit_message>
correct predictions for sgb
</commit_message>
<xml_diff>
--- a/phase_I/CxFPoolsEuro2020_PhaseI_SeanGattBaldacchino.xlsx
+++ b/phase_I/CxFPoolsEuro2020_PhaseI_SeanGattBaldacchino.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lukeaarohi/pyfiles/EURO2020/phase_I/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\seangb\OneDrive - UGL\PC Data\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A71FDC4-C938-394E-8027-19D715A29E2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{120582AF-DB38-41D0-A070-667C9ED11F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="vgG/epmm7NjsTdVwX9iBzIU5shiiCtARjNuWodo7y419AcMSriaq3jDUeRC0n7fHjZPt0I68wN8Tr2jgEo1fyA==" workbookSaltValue="xcDVmDhqHI6MTRUJYwzs1Q==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matches" sheetId="2" r:id="rId1"/>
@@ -714,13 +714,13 @@
     </r>
   </si>
   <si>
-    <t>Phil Foden</t>
-  </si>
-  <si>
     <t>Sean Gatt Baldacchino</t>
   </si>
   <si>
     <t>Romelu Lukaku</t>
+  </si>
+  <si>
+    <t>Kai Havertz</t>
   </si>
 </sst>
 </file>
@@ -3688,40 +3688,40 @@
   <dimension ref="A1:CY69"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B56" sqref="B56:M56"/>
+      <pane ySplit="9" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M62" sqref="M62"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.5" style="13" customWidth="1"/>
-    <col min="2" max="3" width="3.83203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="10.1640625" style="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.83203125" style="14" customWidth="1"/>
-    <col min="6" max="7" width="3.1640625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" style="13" customWidth="1"/>
+    <col min="2" max="3" width="3.77734375" style="14" customWidth="1"/>
+    <col min="4" max="4" width="10.109375" style="23" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.77734375" style="14" customWidth="1"/>
+    <col min="6" max="7" width="3.109375" style="14" customWidth="1"/>
     <col min="8" max="8" width="22" style="14" customWidth="1"/>
     <col min="9" max="9" width="0.6640625" style="14" customWidth="1"/>
-    <col min="10" max="10" width="0.5" style="14" customWidth="1"/>
+    <col min="10" max="10" width="0.44140625" style="14" customWidth="1"/>
     <col min="11" max="11" width="0.6640625" style="14" customWidth="1"/>
-    <col min="12" max="12" width="3.83203125" style="14" customWidth="1"/>
-    <col min="13" max="13" width="17.5" style="14" customWidth="1"/>
-    <col min="14" max="14" width="1.5" style="14" customWidth="1"/>
-    <col min="15" max="20" width="3.83203125" style="14" customWidth="1"/>
-    <col min="21" max="21" width="3.83203125" style="15" customWidth="1"/>
-    <col min="22" max="22" width="3.83203125" style="24" customWidth="1"/>
-    <col min="23" max="24" width="3.83203125" style="14" customWidth="1"/>
-    <col min="25" max="25" width="1.5" style="14" customWidth="1"/>
-    <col min="26" max="28" width="3.83203125" style="14" customWidth="1"/>
-    <col min="29" max="29" width="2.83203125" style="14" customWidth="1"/>
-    <col min="30" max="31" width="3.83203125" style="14" customWidth="1"/>
+    <col min="12" max="12" width="3.77734375" style="14" customWidth="1"/>
+    <col min="13" max="13" width="17.44140625" style="14" customWidth="1"/>
+    <col min="14" max="14" width="1.44140625" style="14" customWidth="1"/>
+    <col min="15" max="20" width="3.77734375" style="14" customWidth="1"/>
+    <col min="21" max="21" width="3.77734375" style="15" customWidth="1"/>
+    <col min="22" max="22" width="3.77734375" style="24" customWidth="1"/>
+    <col min="23" max="24" width="3.77734375" style="14" customWidth="1"/>
+    <col min="25" max="25" width="1.44140625" style="14" customWidth="1"/>
+    <col min="26" max="28" width="3.77734375" style="14" customWidth="1"/>
+    <col min="29" max="29" width="2.77734375" style="14" customWidth="1"/>
+    <col min="30" max="31" width="3.77734375" style="14" customWidth="1"/>
     <col min="32" max="32" width="3" style="14" customWidth="1"/>
-    <col min="33" max="33" width="9.1640625" style="14" customWidth="1"/>
-    <col min="34" max="34" width="9.1640625" style="13" customWidth="1"/>
-    <col min="35" max="97" width="9.1640625" style="14" customWidth="1"/>
-    <col min="98" max="16384" width="9.1640625" style="14"/>
+    <col min="33" max="33" width="9.109375" style="14" customWidth="1"/>
+    <col min="34" max="34" width="9.109375" style="13" customWidth="1"/>
+    <col min="35" max="97" width="9.109375" style="14" customWidth="1"/>
+    <col min="98" max="16384" width="9.109375" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:103" x14ac:dyDescent="0.3">
       <c r="B1" s="244" t="s">
         <v>133</v>
       </c>
@@ -3753,7 +3753,7 @@
       <c r="AB1" s="244"/>
       <c r="AC1" s="244"/>
     </row>
-    <row r="2" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="260" t="s">
         <v>129</v>
       </c>
@@ -3789,7 +3789,7 @@
       <c r="AB2" s="263"/>
       <c r="AC2" s="264"/>
     </row>
-    <row r="3" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="261"/>
       <c r="C3" s="261"/>
       <c r="D3" s="261"/>
@@ -3822,7 +3822,7 @@
       <c r="AB3" s="265"/>
       <c r="AC3" s="266"/>
     </row>
-    <row r="4" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:103" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="261"/>
       <c r="C4" s="261"/>
       <c r="D4" s="261"/>
@@ -3846,7 +3846,7 @@
         <v>109</v>
       </c>
       <c r="U4" s="267" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="V4" s="268"/>
       <c r="W4" s="268"/>
@@ -3857,7 +3857,7 @@
       <c r="AB4" s="268"/>
       <c r="AC4" s="269"/>
     </row>
-    <row r="5" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:103" x14ac:dyDescent="0.3">
       <c r="B5" s="162"/>
       <c r="C5" s="162"/>
       <c r="D5" s="162"/>
@@ -3887,7 +3887,7 @@
       <c r="AB5" s="157"/>
       <c r="AC5" s="201"/>
     </row>
-    <row r="6" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:103" x14ac:dyDescent="0.3">
       <c r="B6" s="162"/>
       <c r="C6" s="162"/>
       <c r="D6" s="162"/>
@@ -3924,7 +3924,7 @@
       <c r="AH6" s="165"/>
       <c r="AI6" s="165"/>
     </row>
-    <row r="7" spans="1:103" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:103" x14ac:dyDescent="0.3">
       <c r="B7" s="162"/>
       <c r="C7" s="162"/>
       <c r="D7" s="162"/>
@@ -3961,7 +3961,7 @@
       <c r="AH7" s="165"/>
       <c r="AI7" s="165"/>
     </row>
-    <row r="8" spans="1:103" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:103" ht="9" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="162"/>
       <c r="C8" s="162"/>
       <c r="D8" s="162"/>
@@ -3975,7 +3975,7 @@
       <c r="AD8" s="166"/>
       <c r="AI8" s="167"/>
     </row>
-    <row r="9" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="16">
         <v>7</v>
       </c>
@@ -4030,7 +4030,7 @@
       <c r="AH9" s="16"/>
       <c r="CY9" s="14"/>
     </row>
-    <row r="10" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="16">
         <f>MAX(A11:A62)</f>
         <v>3</v>
@@ -4091,7 +4091,7 @@
       </c>
       <c r="CY10" s="14"/>
     </row>
-    <row r="11" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="37">
         <v>1</v>
@@ -4179,7 +4179,7 @@
       </c>
       <c r="CY11" s="14"/>
     </row>
-    <row r="12" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="16"/>
       <c r="B12" s="46">
         <v>2</v>
@@ -4265,7 +4265,7 @@
       </c>
       <c r="CY12" s="14"/>
     </row>
-    <row r="13" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="46">
         <v>3</v>
@@ -4313,11 +4313,11 @@
       </c>
       <c r="U13" s="54">
         <f>VLOOKUP(P13,'Dummy Table'!B4:C40,2,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13" s="54">
         <f>VLOOKUP(P13,'Dummy Table'!B4:D40,3,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="W13" s="54">
         <f>VLOOKUP(P13,'Dummy Table'!B4:E40,4,FALSE)</f>
@@ -4325,7 +4325,7 @@
       </c>
       <c r="X13" s="54">
         <f>VLOOKUP(P13,'Dummy Table'!B4:F40,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y13" s="54" t="s">
         <v>45</v>
@@ -4336,11 +4336,11 @@
       </c>
       <c r="AA13" s="54">
         <f>X13-Z13</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="AB13" s="54">
         <f>U13*3+V13*1</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AC13" s="168"/>
       <c r="AD13" s="31"/>
@@ -4351,7 +4351,7 @@
       </c>
       <c r="CY13" s="14"/>
     </row>
-    <row r="14" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="46">
         <v>4</v>
@@ -4403,11 +4403,11 @@
       </c>
       <c r="V14" s="55">
         <f>VLOOKUP(P14,'Dummy Table'!B4:D40,3,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W14" s="55">
         <f>VLOOKUP(P14,'Dummy Table'!B4:E40,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X14" s="55">
         <f>VLOOKUP(P14,'Dummy Table'!B4:F40,5,FALSE)</f>
@@ -4418,15 +4418,15 @@
       </c>
       <c r="Z14" s="55">
         <f>VLOOKUP(P14,'Dummy Table'!B4:G40,6,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AA14" s="55">
         <f>X14-Z14</f>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="AB14" s="55">
         <f>U14*3+V14*1</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="168"/>
       <c r="AD14" s="31"/>
@@ -4437,7 +4437,7 @@
       </c>
       <c r="CY14" s="14"/>
     </row>
-    <row r="15" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="46">
         <v>5</v>
@@ -4510,7 +4510,7 @@
       </c>
       <c r="CY15" s="14"/>
     </row>
-    <row r="16" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="46">
         <v>6</v>
@@ -4596,7 +4596,7 @@
       </c>
       <c r="CY16" s="14"/>
     </row>
-    <row r="17" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="46">
         <v>7</v>
@@ -4682,7 +4682,7 @@
       </c>
       <c r="CY17" s="14"/>
     </row>
-    <row r="18" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="46">
         <v>8</v>
@@ -4768,7 +4768,7 @@
       </c>
       <c r="CY18" s="14"/>
     </row>
-    <row r="19" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="46">
         <v>9</v>
@@ -4854,7 +4854,7 @@
       </c>
       <c r="CY19" s="14"/>
     </row>
-    <row r="20" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="46">
         <v>10</v>
@@ -4927,7 +4927,7 @@
       </c>
       <c r="CY20" s="14"/>
     </row>
-    <row r="21" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="46">
         <v>11</v>
@@ -5013,7 +5013,7 @@
       </c>
       <c r="CY21" s="14"/>
     </row>
-    <row r="22" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A22" s="16">
         <f>IF(F22&lt;&gt;"",1,0)</f>
         <v>1</v>
@@ -5064,11 +5064,11 @@
       </c>
       <c r="U22" s="70">
         <f>VLOOKUP(P22,'Dummy Table'!B4:C40,2,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V22" s="70">
         <f>VLOOKUP(P22,'Dummy Table'!B4:D40,3,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W22" s="70">
         <f>VLOOKUP(P22,'Dummy Table'!B4:E40,4,FALSE)</f>
@@ -5076,7 +5076,7 @@
       </c>
       <c r="X22" s="70">
         <f>VLOOKUP(P22,'Dummy Table'!B4:F40,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Y22" s="70" t="s">
         <v>45</v>
@@ -5087,11 +5087,11 @@
       </c>
       <c r="AA22" s="70">
         <f>X22-Z22</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB22" s="70">
         <f>U22*3+V22*1</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AC22" s="168"/>
       <c r="AD22" s="31"/>
@@ -5102,7 +5102,7 @@
       </c>
       <c r="CY22" s="14"/>
     </row>
-    <row r="23" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="71">
         <v>13</v>
@@ -5156,11 +5156,11 @@
       </c>
       <c r="V23" s="78">
         <f>VLOOKUP(P23,'Dummy Table'!B4:D40,3,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W23" s="78">
         <f>VLOOKUP(P23,'Dummy Table'!B4:E40,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X23" s="78">
         <f>VLOOKUP(P23,'Dummy Table'!B4:F40,5,FALSE)</f>
@@ -5171,15 +5171,15 @@
       </c>
       <c r="Z23" s="78">
         <f>VLOOKUP(P23,'Dummy Table'!B4:G40,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA23" s="78">
         <f>X23-Z23</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="AB23" s="78">
         <f>U23*3+V23*1</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AC23" s="168"/>
       <c r="AD23" s="31"/>
@@ -5190,7 +5190,7 @@
       </c>
       <c r="CY23" s="14"/>
     </row>
-    <row r="24" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="79">
         <v>14</v>
@@ -5276,7 +5276,7 @@
       </c>
       <c r="CY24" s="14"/>
     </row>
-    <row r="25" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="79">
         <v>15</v>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="CY25" s="14"/>
     </row>
-    <row r="26" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="79">
         <v>16</v>
@@ -5435,7 +5435,7 @@
       </c>
       <c r="CY26" s="14"/>
     </row>
-    <row r="27" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="79">
         <v>17</v>
@@ -5521,7 +5521,7 @@
       </c>
       <c r="CY27" s="14"/>
     </row>
-    <row r="28" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="16"/>
       <c r="B28" s="79">
         <v>18</v>
@@ -5607,7 +5607,7 @@
       </c>
       <c r="CY28" s="14"/>
     </row>
-    <row r="29" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="16"/>
       <c r="B29" s="79">
         <v>19</v>
@@ -5693,7 +5693,7 @@
       </c>
       <c r="CY29" s="14"/>
     </row>
-    <row r="30" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="16"/>
       <c r="B30" s="79">
         <v>20</v>
@@ -5766,7 +5766,7 @@
       </c>
       <c r="CY30" s="14"/>
     </row>
-    <row r="31" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="16"/>
       <c r="B31" s="79">
         <v>21</v>
@@ -5852,7 +5852,7 @@
       </c>
       <c r="CY31" s="14"/>
     </row>
-    <row r="32" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="16"/>
       <c r="B32" s="79">
         <v>22</v>
@@ -5938,7 +5938,7 @@
       </c>
       <c r="CY32" s="14"/>
     </row>
-    <row r="33" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="16"/>
       <c r="B33" s="79">
         <v>23</v>
@@ -6024,7 +6024,7 @@
       </c>
       <c r="CY33" s="14"/>
     </row>
-    <row r="34" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A34" s="16">
         <f>IF(F34&lt;&gt;"",2,0)</f>
         <v>2</v>
@@ -6110,7 +6110,7 @@
       <c r="AH34" s="16"/>
       <c r="CY34" s="14"/>
     </row>
-    <row r="35" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="16"/>
       <c r="B35" s="206">
         <v>25</v>
@@ -6128,7 +6128,7 @@
         <v>1</v>
       </c>
       <c r="G35" s="210">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H35" s="211" t="s">
         <v>24</v>
@@ -6141,7 +6141,7 @@
       </c>
       <c r="M35" s="102" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Turkey</v>
       </c>
       <c r="N35" s="31"/>
       <c r="O35" s="248" t="s">
@@ -6182,7 +6182,7 @@
       <c r="AH35" s="16"/>
       <c r="CY35" s="14"/>
     </row>
-    <row r="36" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="16"/>
       <c r="B36" s="46">
         <v>26</v>
@@ -6265,7 +6265,7 @@
       <c r="AH36" s="16"/>
       <c r="CY36" s="14"/>
     </row>
-    <row r="37" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="16"/>
       <c r="B37" s="46">
         <v>27</v>
@@ -6348,7 +6348,7 @@
       <c r="AH37" s="16"/>
       <c r="CY37" s="14"/>
     </row>
-    <row r="38" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="16"/>
       <c r="B38" s="46">
         <v>28</v>
@@ -6363,7 +6363,7 @@
         <v>25</v>
       </c>
       <c r="F38" s="185">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G38" s="185">
         <v>0</v>
@@ -6377,7 +6377,7 @@
       <c r="L38" s="242"/>
       <c r="M38" s="52" t="str">
         <f t="shared" si="0"/>
-        <v/>
+        <v>Ukraine</v>
       </c>
       <c r="N38" s="31"/>
       <c r="O38" s="132">
@@ -6431,7 +6431,7 @@
       <c r="AH38" s="16"/>
       <c r="CY38" s="14"/>
     </row>
-    <row r="39" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="16"/>
       <c r="B39" s="46">
         <v>29</v>
@@ -6514,7 +6514,7 @@
       <c r="AH39" s="16"/>
       <c r="CY39" s="14"/>
     </row>
-    <row r="40" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="16"/>
       <c r="B40" s="46">
         <v>30</v>
@@ -6566,7 +6566,7 @@
       <c r="AH40" s="16"/>
       <c r="CY40" s="14"/>
     </row>
-    <row r="41" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="16"/>
       <c r="B41" s="46">
         <v>31</v>
@@ -6620,7 +6620,7 @@
       <c r="AH41" s="16"/>
       <c r="CY41" s="14"/>
     </row>
-    <row r="42" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="16"/>
       <c r="B42" s="46">
         <v>32</v>
@@ -6692,7 +6692,7 @@
       <c r="AH42" s="16"/>
       <c r="CY42" s="14"/>
     </row>
-    <row r="43" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="16"/>
       <c r="B43" s="46">
         <v>33</v>
@@ -6778,7 +6778,7 @@
       <c r="AH43" s="16"/>
       <c r="CY43" s="14"/>
     </row>
-    <row r="44" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="16"/>
       <c r="B44" s="46">
         <v>34</v>
@@ -6815,7 +6815,7 @@
       </c>
       <c r="P44" s="285" t="str">
         <f>INDEX('Dummy Table'!DH3:DH8,MATCH(Matches!O44,'Dummy Table'!DU3:DU8,0),0)</f>
-        <v>Austria</v>
+        <v>Turkey</v>
       </c>
       <c r="Q44" s="285"/>
       <c r="R44" s="285"/>
@@ -6838,14 +6838,14 @@
       </c>
       <c r="X44" s="111">
         <f>VLOOKUP(P44,P11:AB39,9,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y44" s="111" t="s">
         <v>45</v>
       </c>
       <c r="Z44" s="111">
         <f>VLOOKUP(P44,P11:AB39,11,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AA44" s="111">
         <f>VLOOKUP(P44,P11:AB39,12,FALSE)</f>
@@ -6857,14 +6857,14 @@
       </c>
       <c r="AC44" s="140" t="str">
         <f>INDEX('Dummy Table'!DV3:DV8,MATCH(Matches!O44,'Dummy Table'!DU3:DU8,0),0)</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="AD44" s="31"/>
       <c r="AE44" s="14"/>
       <c r="AH44" s="16"/>
       <c r="CY44" s="14"/>
     </row>
-    <row r="45" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="16"/>
       <c r="B45" s="46">
         <v>35</v>
@@ -6950,7 +6950,7 @@
       <c r="AH45" s="16"/>
       <c r="CY45" s="14"/>
     </row>
-    <row r="46" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="16">
         <f>IF(F46&lt;&gt;"",3,0)</f>
         <v>3</v>
@@ -7039,7 +7039,7 @@
       <c r="AH46" s="16"/>
       <c r="CY46" s="14"/>
     </row>
-    <row r="47" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="16"/>
       <c r="N47" s="31"/>
       <c r="O47" s="141">
@@ -7047,7 +7047,7 @@
       </c>
       <c r="P47" s="278" t="str">
         <f>INDEX('Dummy Table'!DH3:DH8,MATCH(Matches!O47,'Dummy Table'!DU3:DU8,0),0)</f>
-        <v>Scotland</v>
+        <v>Austria</v>
       </c>
       <c r="Q47" s="278"/>
       <c r="R47" s="278"/>
@@ -7070,18 +7070,18 @@
       </c>
       <c r="X47" s="112">
         <f>VLOOKUP(P47,P11:AB39,9,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y47" s="112" t="s">
         <v>45</v>
       </c>
       <c r="Z47" s="112">
         <f>VLOOKUP(P47,P11:AB39,11,FALSE)</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="AA47" s="112">
         <f>VLOOKUP(P47,P11:AB39,12,FALSE)</f>
-        <v>-3</v>
+        <v>-1</v>
       </c>
       <c r="AB47" s="112">
         <f>VLOOKUP(P47,P11:AB39,13,FALSE)</f>
@@ -7089,14 +7089,14 @@
       </c>
       <c r="AC47" s="142" t="str">
         <f>INDEX('Dummy Table'!DV3:DV8,MATCH(Matches!O47,'Dummy Table'!DU3:DU8,0),0)</f>
-        <v>D</v>
+        <v>C</v>
       </c>
       <c r="AD47" s="31"/>
       <c r="AE47" s="14"/>
       <c r="AH47" s="16"/>
       <c r="CY47" s="14"/>
     </row>
-    <row r="48" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:103" s="17" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="16"/>
       <c r="B48" s="231" t="s">
         <v>134</v>
@@ -7118,7 +7118,7 @@
       </c>
       <c r="P48" s="279" t="str">
         <f>INDEX('Dummy Table'!DH3:DH8,MATCH(Matches!O48,'Dummy Table'!DU3:DU8,0),0)</f>
-        <v>Turkey</v>
+        <v>Scotland</v>
       </c>
       <c r="Q48" s="279"/>
       <c r="R48" s="279"/>
@@ -7129,15 +7129,15 @@
       </c>
       <c r="U48" s="144">
         <f>VLOOKUP(P48,P11:AB39,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V48" s="144">
         <f>VLOOKUP(P48,P11:AB39,7,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="W48" s="144">
         <f>VLOOKUP(P48,P11:AB39,8,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X48" s="144">
         <f>VLOOKUP(P48,P11:AB39,9,FALSE)</f>
@@ -7148,29 +7148,29 @@
       </c>
       <c r="Z48" s="144">
         <f>VLOOKUP(P48,P11:AB39,11,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AA48" s="144">
         <f>VLOOKUP(P48,P11:AB39,12,FALSE)</f>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="AB48" s="144">
         <f>VLOOKUP(P48,P11:AB39,13,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AC48" s="145" t="str">
         <f>INDEX('Dummy Table'!DV3:DV8,MATCH(Matches!O48,'Dummy Table'!DU3:DU8,0),0)</f>
-        <v>A</v>
+        <v>D</v>
       </c>
       <c r="AD48" s="31"/>
       <c r="AE48" s="14"/>
       <c r="AH48" s="16"/>
       <c r="CV48" s="14"/>
     </row>
-    <row r="49" spans="1:96" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:96" s="17" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="16"/>
       <c r="B49" s="217" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="C49" s="218"/>
       <c r="D49" s="218"/>
@@ -7204,10 +7204,10 @@
       <c r="AH49" s="16"/>
       <c r="CR49" s="14"/>
     </row>
-    <row r="50" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="16"/>
       <c r="B50" s="237" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C50" s="238"/>
       <c r="D50" s="238"/>
@@ -7246,9 +7246,9 @@
       <c r="AI50" s="17"/>
       <c r="AJ50" s="17"/>
     </row>
-    <row r="51" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B51" s="237" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="C51" s="238"/>
       <c r="D51" s="238"/>
@@ -7281,9 +7281,9 @@
       <c r="AC51" s="246"/>
       <c r="AD51" s="247"/>
     </row>
-    <row r="52" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B52" s="214" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C52" s="215"/>
       <c r="D52" s="215"/>
@@ -7314,7 +7314,7 @@
       <c r="AC52" s="246"/>
       <c r="AD52" s="247"/>
     </row>
-    <row r="53" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N53" s="21"/>
       <c r="O53" s="170">
         <v>1</v>
@@ -7337,7 +7337,7 @@
       <c r="AC53" s="115"/>
       <c r="AD53" s="117"/>
     </row>
-    <row r="54" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B54" s="231" t="s">
         <v>135</v>
       </c>
@@ -7374,7 +7374,7 @@
       <c r="AC54" s="171"/>
       <c r="AD54" s="173"/>
     </row>
-    <row r="55" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="16"/>
       <c r="B55" s="217" t="s">
         <v>10</v>
@@ -7412,7 +7412,7 @@
       <c r="AC55" s="171"/>
       <c r="AD55" s="173"/>
     </row>
-    <row r="56" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B56" s="214" t="s">
         <v>8</v>
       </c>
@@ -7447,7 +7447,7 @@
       <c r="AC56" s="246"/>
       <c r="AD56" s="247"/>
     </row>
-    <row r="57" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N57" s="21"/>
       <c r="O57" s="245"/>
       <c r="P57" s="246"/>
@@ -7466,7 +7466,7 @@
       <c r="AC57" s="246"/>
       <c r="AD57" s="247"/>
     </row>
-    <row r="58" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B58" s="234" t="s">
         <v>114</v>
       </c>
@@ -7503,7 +7503,7 @@
       <c r="AC58" s="171"/>
       <c r="AD58" s="173"/>
     </row>
-    <row r="59" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="16"/>
       <c r="B59" s="229" t="s">
         <v>10</v>
@@ -7541,7 +7541,7 @@
       <c r="AC59" s="171"/>
       <c r="AD59" s="173"/>
     </row>
-    <row r="60" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:96" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="N60" s="21"/>
       <c r="O60" s="170">
         <v>6</v>
@@ -7564,7 +7564,7 @@
       <c r="AC60" s="171"/>
       <c r="AD60" s="173"/>
     </row>
-    <row r="61" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="16"/>
       <c r="B61" s="226" t="s">
         <v>113</v>
@@ -7602,7 +7602,7 @@
       <c r="AC61" s="171"/>
       <c r="AD61" s="173"/>
     </row>
-    <row r="62" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="16"/>
       <c r="B62" s="176">
         <v>1</v>
@@ -7620,7 +7620,7 @@
       <c r="K62" s="177"/>
       <c r="L62" s="177"/>
       <c r="M62" s="114" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="N62" s="21"/>
       <c r="O62" s="170">
@@ -7644,7 +7644,7 @@
       <c r="AC62" s="115"/>
       <c r="AD62" s="117"/>
     </row>
-    <row r="63" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:96" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="16"/>
       <c r="B63" s="176">
         <v>2</v>
@@ -7662,7 +7662,7 @@
       <c r="K63" s="177"/>
       <c r="L63" s="177"/>
       <c r="M63" s="114" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="N63" s="175"/>
       <c r="O63" s="220" t="s">
@@ -7684,7 +7684,7 @@
       <c r="AC63" s="221"/>
       <c r="AD63" s="222"/>
     </row>
-    <row r="64" spans="1:96" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:96" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="14"/>
       <c r="B64" s="178">
         <v>3</v>
@@ -7702,7 +7702,7 @@
       <c r="K64" s="180"/>
       <c r="L64" s="180"/>
       <c r="M64" s="213" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="N64" s="175"/>
       <c r="O64" s="223"/>
@@ -7723,7 +7723,7 @@
       <c r="AD64" s="225"/>
       <c r="AH64" s="14"/>
     </row>
-    <row r="65" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A65" s="14"/>
       <c r="N65" s="175"/>
       <c r="O65" s="182"/>
@@ -7744,7 +7744,7 @@
       <c r="AD65" s="182"/>
       <c r="AH65" s="14"/>
     </row>
-    <row r="66" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A66" s="14"/>
       <c r="N66" s="175"/>
       <c r="O66" s="182"/>
@@ -7765,7 +7765,7 @@
       <c r="AD66" s="182"/>
       <c r="AH66" s="14"/>
     </row>
-    <row r="67" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:34" x14ac:dyDescent="0.3">
       <c r="N67" s="175"/>
       <c r="O67" s="182"/>
       <c r="P67" s="182"/>
@@ -7784,16 +7784,15 @@
       <c r="AC67" s="182"/>
       <c r="AD67" s="182"/>
     </row>
-    <row r="68" spans="1:34" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:34" x14ac:dyDescent="0.3">
       <c r="N68" s="175"/>
     </row>
-    <row r="69" spans="1:34" ht="16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="N69" s="181"/>
     </row>
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="R0u/bZzfvofvHo9HKAqllZcKVNwD4Pqz++sozZh+LmARazUyfNjXbD6MLNyOAVxsvOWLG/EqcCF3JT4/IQtMAA==" saltValue="vbEGenma5H7Im9k/JMzelA==" spinCount="100000" sheet="1" selectLockedCells="1"/>
   <mergeCells count="61">
-    <mergeCell ref="B51:M51"/>
     <mergeCell ref="O30:S30"/>
     <mergeCell ref="P31:S31"/>
     <mergeCell ref="P33:S33"/>
@@ -7845,6 +7844,7 @@
     <mergeCell ref="B48:M48"/>
     <mergeCell ref="B49:M49"/>
     <mergeCell ref="B50:M50"/>
+    <mergeCell ref="B51:M51"/>
     <mergeCell ref="I3:N4"/>
     <mergeCell ref="L11:L22"/>
     <mergeCell ref="B52:M52"/>
@@ -7928,418 +7928,418 @@
       <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.1640625" style="192" bestFit="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.1640625" style="183"/>
+    <col min="1" max="1" width="23.109375" style="192" bestFit="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.109375" style="183"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="188" t="str">
         <f>Matches!U4</f>
         <v>Sean Gatt Baldacchino</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="189" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="190" t="str">
         <f>TEXT(Matches!F11,"#0")&amp;"-"&amp;TEXT(Matches!G11,"#0")</f>
         <v>0-1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="190" t="str">
         <f>TEXT(Matches!F12,"#0")&amp;"-"&amp;TEXT(Matches!G12,"#0")</f>
         <v>1-0</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="190" t="str">
         <f>TEXT(Matches!F13,"#0")&amp;"-"&amp;TEXT(Matches!G13,"#0")</f>
         <v>2-0</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="190" t="str">
         <f>TEXT(Matches!F14,"#0")&amp;"-"&amp;TEXT(Matches!G14,"#0")</f>
         <v>3-0</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="190" t="str">
         <f>TEXT(Matches!F15,"#0")&amp;"-"&amp;TEXT(Matches!G15,"#0")</f>
         <v>1-1</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="190" t="str">
         <f>TEXT(Matches!F16,"#0")&amp;"-"&amp;TEXT(Matches!G16,"#0")</f>
         <v>1-0</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="190" t="str">
         <f>TEXT(Matches!F17,"#0")&amp;"-"&amp;TEXT(Matches!G17,"#0")</f>
         <v>2-1</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A10" s="190" t="str">
         <f>TEXT(Matches!F18,"#0")&amp;"-"&amp;TEXT(Matches!G18,"#0")</f>
         <v>1-0</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A11" s="190" t="str">
         <f>TEXT(Matches!F19,"#0")&amp;"-"&amp;TEXT(Matches!G19,"#0")</f>
         <v>1-0</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="190" t="str">
         <f>TEXT(Matches!F20,"#0")&amp;"-"&amp;TEXT(Matches!G20,"#0")</f>
         <v>2-0</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="190" t="str">
         <f>TEXT(Matches!F21,"#0")&amp;"-"&amp;TEXT(Matches!G21,"#0")</f>
         <v>0-1</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="190" t="str">
         <f>TEXT(Matches!F22,"#0")&amp;"-"&amp;TEXT(Matches!G22,"#0")</f>
         <v>2-1</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="190" t="str">
         <f>TEXT(Matches!F23,"#0")&amp;"-"&amp;TEXT(Matches!G23,"#0")</f>
         <v>0-1</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A16" s="190" t="str">
         <f>TEXT(Matches!F24,"#0")&amp;"-"&amp;TEXT(Matches!G24,"#0")</f>
         <v>1-1</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" s="190" t="str">
         <f>TEXT(Matches!F25,"#0")&amp;"-"&amp;TEXT(Matches!G25,"#0")</f>
         <v>2-0</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="190" t="str">
         <f>TEXT(Matches!F26,"#0")&amp;"-"&amp;TEXT(Matches!G26,"#0")</f>
         <v>1-0</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="190" t="str">
         <f>TEXT(Matches!F27,"#0")&amp;"-"&amp;TEXT(Matches!G27,"#0")</f>
         <v>0-2</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="190" t="str">
         <f>TEXT(Matches!F28,"#0")&amp;"-"&amp;TEXT(Matches!G28,"#0")</f>
         <v>1-0</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="190" t="str">
         <f>TEXT(Matches!F29,"#0")&amp;"-"&amp;TEXT(Matches!G29,"#0")</f>
         <v>1-0</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="190" t="str">
         <f>TEXT(Matches!F30,"#0")&amp;"-"&amp;TEXT(Matches!G30,"#0")</f>
         <v>2-0</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="190" t="str">
         <f>TEXT(Matches!F31,"#0")&amp;"-"&amp;TEXT(Matches!G31,"#0")</f>
         <v>3-0</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="190" t="str">
         <f>TEXT(Matches!F32,"#0")&amp;"-"&amp;TEXT(Matches!G32,"#0")</f>
         <v>0-2</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="190" t="str">
         <f>TEXT(Matches!F33,"#0")&amp;"-"&amp;TEXT(Matches!G33,"#0")</f>
         <v>1-1</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" s="190" t="str">
         <f>TEXT(Matches!F34,"#0")&amp;"-"&amp;TEXT(Matches!G34,"#0")</f>
         <v>2-0</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="190" t="str">
         <f>TEXT(Matches!F35,"#0")&amp;"-"&amp;TEXT(Matches!G35,"#0")</f>
-        <v>1-1</v>
+        <v>1-2</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" s="190" t="str">
         <f>TEXT(Matches!F36,"#0")&amp;"-"&amp;TEXT(Matches!G36,"#0")</f>
         <v>1-1</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" s="190" t="str">
         <f>TEXT(Matches!F37,"#0")&amp;"-"&amp;TEXT(Matches!G37,"#0")</f>
         <v>0-2</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="190" t="str">
         <f>TEXT(Matches!F38,"#0")&amp;"-"&amp;TEXT(Matches!G38,"#0")</f>
-        <v>0-0</v>
+        <v>1-0</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="190" t="str">
         <f>TEXT(Matches!F39,"#0")&amp;"-"&amp;TEXT(Matches!G39,"#0")</f>
         <v>0-0</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" s="190" t="str">
         <f>TEXT(Matches!F40,"#0")&amp;"-"&amp;TEXT(Matches!G40,"#0")</f>
         <v>0-4</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A33" s="190" t="str">
         <f>TEXT(Matches!F41,"#0")&amp;"-"&amp;TEXT(Matches!G41,"#0")</f>
         <v>2-1</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A34" s="190" t="str">
         <f>TEXT(Matches!F42,"#0")&amp;"-"&amp;TEXT(Matches!G42,"#0")</f>
         <v>0-2</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A35" s="190" t="str">
         <f>TEXT(Matches!F43,"#0")&amp;"-"&amp;TEXT(Matches!G43,"#0")</f>
         <v>1-1</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A36" s="190" t="str">
         <f>TEXT(Matches!F44,"#0")&amp;"-"&amp;TEXT(Matches!G44,"#0")</f>
         <v>0-2</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A37" s="190" t="str">
         <f>TEXT(Matches!F45,"#0")&amp;"-"&amp;TEXT(Matches!G45,"#0")</f>
         <v>1-2</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="190" t="str">
         <f>TEXT(Matches!F46,"#0")&amp;"-"&amp;TEXT(Matches!G46,"#0")</f>
         <v>3-0</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="191" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" s="190" t="str">
         <f>Matches!P11</f>
         <v>Italy</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" s="190" t="str">
         <f>Matches!P12</f>
         <v>Wales</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" s="190" t="str">
         <f>Matches!P16</f>
         <v>Belgium</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" s="190" t="str">
         <f>Matches!P17</f>
         <v>Denmark</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" s="190" t="str">
         <f>Matches!P21</f>
         <v>Netherlands</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" s="190" t="str">
         <f>Matches!P22</f>
         <v>Ukraine</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" s="190" t="str">
         <f>Matches!P26</f>
         <v>England</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" s="190" t="str">
         <f>Matches!P27</f>
         <v>Croatia</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" s="190" t="str">
         <f>Matches!P31</f>
         <v>Spain</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" s="190" t="str">
         <f>Matches!P32</f>
         <v>Poland</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" s="190" t="str">
         <f>Matches!P36</f>
         <v>France</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" s="190" t="str">
         <f>Matches!P37</f>
         <v>Germany</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A52" s="190" t="str">
         <f>Matches!P43</f>
         <v>Portugal</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A53" s="190" t="str">
         <f>Matches!P44</f>
-        <v>Austria</v>
+        <v>Turkey</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A54" s="190" t="str">
         <f>Matches!P45</f>
         <v>Sweden</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A55" s="190" t="str">
         <f>Matches!P46</f>
         <v>Russia</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A56" s="191" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A57" s="190" t="str">
         <f>Matches!B49</f>
-        <v>France</v>
+        <v>Portugal</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A58" s="190" t="str">
         <f>Matches!B50</f>
-        <v>Belgium</v>
+        <v>France</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A59" s="190" t="str">
         <f>Matches!B51</f>
-        <v>Italy</v>
+        <v>England</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A60" s="190" t="str">
         <f>Matches!B52</f>
-        <v>England</v>
+        <v>Belgium</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A61" s="191" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A62" s="190" t="str">
         <f>Matches!B55</f>
         <v>France</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A63" s="190" t="str">
         <f>Matches!B56</f>
         <v>England</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A64" s="191" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" s="190" t="str">
         <f>Matches!B59</f>
         <v>France</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" s="191" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" s="190" t="str">
         <f>Matches!M62</f>
-        <v>France</v>
+        <v>Belgium</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" s="190" t="str">
         <f>Matches!M63</f>
         <v>Romelu Lukaku</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" s="190" t="str">
         <f>Matches!M64</f>
-        <v>Phil Foden</v>
+        <v>Kai Havertz</v>
       </c>
     </row>
   </sheetData>
@@ -8362,22 +8362,22 @@
       <selection pane="bottomLeft" activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="3.5" customWidth="1"/>
-    <col min="3" max="3" width="21.5" customWidth="1"/>
-    <col min="4" max="4" width="1.5" customWidth="1"/>
-    <col min="5" max="5" width="2.5" customWidth="1"/>
-    <col min="6" max="6" width="24.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.77734375" customWidth="1"/>
+    <col min="2" max="2" width="3.44140625" customWidth="1"/>
+    <col min="3" max="3" width="21.44140625" customWidth="1"/>
+    <col min="4" max="4" width="1.44140625" customWidth="1"/>
+    <col min="5" max="5" width="2.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="3" customWidth="1"/>
     <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="8.83203125" customWidth="1"/>
-    <col min="11" max="11" width="2.5" customWidth="1"/>
+    <col min="9" max="10" width="8.77734375" customWidth="1"/>
+    <col min="11" max="11" width="2.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="1" customFormat="1" ht="5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="2" spans="1:16" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="4.95" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:16" s="4" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2"/>
       <c r="B2" s="3" t="s">
         <v>0</v>
@@ -8391,11 +8391,11 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:16" ht="5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" ht="4.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="I3" s="5"/>
       <c r="J3" s="5"/>
     </row>
-    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -8413,7 +8413,7 @@
       <c r="O4" s="12"/>
       <c r="P4" s="12"/>
     </row>
-    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="9">
         <v>1</v>
       </c>
@@ -8433,7 +8433,7 @@
       <c r="O5" s="12"/>
       <c r="P5" s="12"/>
     </row>
-    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>2</v>
       </c>
@@ -8453,7 +8453,7 @@
       <c r="O6" s="12"/>
       <c r="P6" s="12"/>
     </row>
-    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="9">
         <v>3</v>
       </c>
@@ -8473,7 +8473,7 @@
       <c r="O7" s="12"/>
       <c r="P7" s="12"/>
     </row>
-    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>4</v>
       </c>
@@ -8493,7 +8493,7 @@
       <c r="O8" s="12"/>
       <c r="P8" s="12"/>
     </row>
-    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="9">
         <v>5</v>
       </c>
@@ -8513,7 +8513,7 @@
       <c r="O9" s="12"/>
       <c r="P9" s="12"/>
     </row>
-    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="9">
         <v>6</v>
       </c>
@@ -8533,7 +8533,7 @@
       <c r="O10" s="12"/>
       <c r="P10" s="12"/>
     </row>
-    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>7</v>
       </c>
@@ -8553,7 +8553,7 @@
       <c r="O11" s="12"/>
       <c r="P11" s="12"/>
     </row>
-    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>8</v>
       </c>
@@ -8573,7 +8573,7 @@
       <c r="O12" s="12"/>
       <c r="P12" s="12"/>
     </row>
-    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>9</v>
       </c>
@@ -8593,7 +8593,7 @@
       <c r="O13" s="290"/>
       <c r="P13" s="290"/>
     </row>
-    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="9">
         <v>10</v>
       </c>
@@ -8613,7 +8613,7 @@
       <c r="O14" s="290"/>
       <c r="P14" s="290"/>
     </row>
-    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="9">
         <v>11</v>
       </c>
@@ -8633,7 +8633,7 @@
       <c r="O15" s="12"/>
       <c r="P15" s="12"/>
     </row>
-    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="9">
         <v>12</v>
       </c>
@@ -8653,7 +8653,7 @@
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
     </row>
-    <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="9">
         <v>13</v>
       </c>
@@ -8673,7 +8673,7 @@
       <c r="O17" s="12"/>
       <c r="P17" s="12"/>
     </row>
-    <row r="18" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="9">
         <v>14</v>
       </c>
@@ -8693,7 +8693,7 @@
       <c r="O18" s="12"/>
       <c r="P18" s="12"/>
     </row>
-    <row r="19" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="9">
         <v>15</v>
       </c>
@@ -8713,7 +8713,7 @@
       <c r="O19" s="12"/>
       <c r="P19" s="12"/>
     </row>
-    <row r="20" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="9">
         <v>16</v>
       </c>
@@ -8733,7 +8733,7 @@
       <c r="O20" s="12"/>
       <c r="P20" s="12"/>
     </row>
-    <row r="21" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="9">
         <v>17</v>
       </c>
@@ -8753,7 +8753,7 @@
       <c r="O21" s="290"/>
       <c r="P21" s="290"/>
     </row>
-    <row r="22" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="9">
         <v>18</v>
       </c>
@@ -8773,7 +8773,7 @@
       <c r="O22" s="290"/>
       <c r="P22" s="290"/>
     </row>
-    <row r="23" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="9">
         <v>19</v>
       </c>
@@ -8793,7 +8793,7 @@
       <c r="O23" s="12"/>
       <c r="P23" s="12"/>
     </row>
-    <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="9">
         <v>20</v>
       </c>
@@ -8813,7 +8813,7 @@
       <c r="O24" s="12"/>
       <c r="P24" s="12"/>
     </row>
-    <row r="25" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="9">
         <v>21</v>
       </c>
@@ -8833,7 +8833,7 @@
       <c r="O25" s="12"/>
       <c r="P25" s="12"/>
     </row>
-    <row r="26" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="9">
         <v>22</v>
       </c>
@@ -8853,7 +8853,7 @@
       <c r="O26" s="12"/>
       <c r="P26" s="12"/>
     </row>
-    <row r="27" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="9">
         <v>23</v>
       </c>
@@ -8873,7 +8873,7 @@
       <c r="O27" s="12"/>
       <c r="P27" s="12"/>
     </row>
-    <row r="28" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="9">
         <v>24</v>
       </c>
@@ -8893,20 +8893,20 @@
       <c r="O28" s="12"/>
       <c r="P28" s="12"/>
     </row>
-    <row r="29" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F29" s="11"/>
       <c r="G29" s="11"/>
       <c r="H29" s="11"/>
       <c r="I29" s="11"/>
     </row>
-    <row r="30" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E30" s="8"/>
     </row>
-    <row r="31" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E31" s="19"/>
       <c r="F31" s="18"/>
     </row>
-    <row r="32" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:16" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
       <c r="G32" s="22"/>
@@ -8919,80 +8919,80 @@
       <c r="N32" s="22"/>
       <c r="O32" s="22"/>
     </row>
-    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="34" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="35" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="36" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="37" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="38" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="39" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="40" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="41" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="42" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="43" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="44" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="45" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="46" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="47" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="48" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="49" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="50" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="51" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="52" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="53" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="54" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="55" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="56" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="57" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="58" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="59" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="60" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="61" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="62" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="63" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="64" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="65" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="66" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="67" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="68" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="81" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="82" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="83" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="84" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="85" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="86" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="87" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="88" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="89" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="90" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="91" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="92" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="93" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="94" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="95" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="96" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="H102" s="10"/>
     </row>
-    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>27</v>
       </c>
@@ -9016,17 +9016,17 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="112" width="8.83203125" style="194" customWidth="1"/>
-    <col min="113" max="119" width="8.83203125" style="200" customWidth="1"/>
-    <col min="120" max="240" width="8.83203125" style="194" customWidth="1"/>
-    <col min="241" max="247" width="8.83203125" style="200" customWidth="1"/>
-    <col min="248" max="256" width="8.83203125" style="194" customWidth="1"/>
-    <col min="257" max="16384" width="9.1640625" style="194"/>
+    <col min="1" max="112" width="8.77734375" style="194" customWidth="1"/>
+    <col min="113" max="119" width="8.77734375" style="200" customWidth="1"/>
+    <col min="120" max="240" width="8.77734375" style="194" customWidth="1"/>
+    <col min="241" max="247" width="8.77734375" style="200" customWidth="1"/>
+    <col min="248" max="256" width="8.77734375" style="194" customWidth="1"/>
+    <col min="257" max="16384" width="9.109375" style="194"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A1" s="21">
         <v>1</v>
       </c>
@@ -9291,7 +9291,7 @@
       <c r="IU1" s="21"/>
       <c r="IV1" s="21"/>
     </row>
-    <row r="2" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="21"/>
@@ -9597,7 +9597,7 @@
       <c r="IU2" s="21"/>
       <c r="IV2" s="21"/>
     </row>
-    <row r="3" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A3" s="21"/>
       <c r="B3" s="21"/>
       <c r="C3" s="21" t="s">
@@ -9915,11 +9915,11 @@
       </c>
       <c r="DI3" s="193">
         <f>Matches!U13</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DJ3" s="193">
         <f>Matches!V13</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DK3" s="193">
         <f>Matches!W13</f>
@@ -9927,7 +9927,7 @@
       </c>
       <c r="DL3" s="193">
         <f>Matches!X13</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="DM3" s="193">
         <f>Matches!Z13</f>
@@ -9935,11 +9935,11 @@
       </c>
       <c r="DN3" s="193">
         <f>Matches!AA13</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="DO3" s="193">
         <f>Matches!AB13</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="DP3" s="21">
         <f>VLOOKUP(DH3,B4:J40,9,FALSE)</f>
@@ -9947,7 +9947,7 @@
       </c>
       <c r="DQ3" s="21">
         <f>RANK(DO3,DO3:DO8)</f>
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="DR3" s="21">
         <f>SUMPRODUCT((DQ3:DQ8=DQ3)*(DN3:DN8&gt;DN3))</f>
@@ -9959,11 +9959,11 @@
       </c>
       <c r="DT3" s="21">
         <f>SUMPRODUCT((DQ3:DQ8=DQ3)*(DN3:DN8=DN3)*(DL3:DL8=DL3)*(DP3:DP8&gt;DP3))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DU3" s="21">
         <f>SUM(DQ3:DT3)</f>
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="DV3" s="21" t="s">
         <v>42</v>
@@ -10101,7 +10101,7 @@
       <c r="IU3" s="21"/>
       <c r="IV3" s="21"/>
     </row>
-    <row r="4" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A4" s="21">
         <f>VLOOKUP(B4,CW4:CX8,2,FALSE)</f>
         <v>3</v>
@@ -10112,11 +10112,11 @@
       </c>
       <c r="C4" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B4)*(DD3:DD42="W"))+SUMPRODUCT((DC3:DC42=B4)*(DE3:DE42="W"))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B4)*(DD3:DD42="D"))+SUMPRODUCT((DC3:DC42=B4)*(DE3:DE42="D"))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B4)*(DD3:DD42="L"))+SUMPRODUCT((DC3:DC42=B4)*(DE3:DE42="L"))</f>
@@ -10124,7 +10124,7 @@
       </c>
       <c r="F4" s="21">
         <f>SUMIF(CZ3:CZ60,B4,DA3:DA60)+SUMIF(DC3:DC60,B4,DB3:DB60)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G4" s="21">
         <f>SUMIF(DC3:DC60,B4,DA3:DA60)+SUMIF(CZ3:CZ60,B4,DB3:DB60)</f>
@@ -10132,11 +10132,11 @@
       </c>
       <c r="H4" s="21">
         <f>F4-G4+1000</f>
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="I4" s="21">
         <f>C4*3+D4*1</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J4" s="21">
         <v>42</v>
@@ -10543,7 +10543,7 @@
       <c r="IU4" s="21"/>
       <c r="IV4" s="21"/>
     </row>
-    <row r="5" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A5" s="21">
         <f>VLOOKUP(B5,CW4:CX8,2,FALSE)</f>
         <v>1</v>
@@ -10863,11 +10863,11 @@
       </c>
       <c r="DJ5" s="193">
         <f>Matches!V23</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DK5" s="193">
         <f>Matches!W23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DL5" s="193">
         <f>Matches!X23</f>
@@ -10875,15 +10875,15 @@
       </c>
       <c r="DM5" s="193">
         <f>Matches!Z23</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DN5" s="193">
         <f>Matches!AA23</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="DO5" s="193">
         <f>Matches!AB23</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="DP5" s="21">
         <f>VLOOKUP(DH5,B4:J40,9,FALSE)</f>
@@ -10891,7 +10891,7 @@
       </c>
       <c r="DQ5" s="21">
         <f>RANK(DO5,DO3:DO8)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="DR5" s="21">
         <f>SUMPRODUCT((DQ3:DQ8=DQ5)*(DN3:DN8&gt;DN5))</f>
@@ -10899,7 +10899,7 @@
       </c>
       <c r="DS5" s="21">
         <f>SUMPRODUCT((DQ3:DQ8=DQ5)*(DN3:DN8=DN5)*(DL3:DL8&gt;DL5))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DT5" s="21">
         <f>SUMPRODUCT((DQ3:DQ8=DQ5)*(DN3:DN8=DN5)*(DL3:DL8=DL5)*(DP3:DP8&gt;DP5))</f>
@@ -10907,7 +10907,7 @@
       </c>
       <c r="DU5" s="21">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="DV5" s="21" t="s">
         <v>48</v>
@@ -11045,7 +11045,7 @@
       <c r="IU5" s="21"/>
       <c r="IV5" s="21"/>
     </row>
-    <row r="6" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A6" s="21">
         <f>VLOOKUP(B6,CW4:CX8,2,FALSE)</f>
         <v>2</v>
@@ -11454,7 +11454,7 @@
       </c>
       <c r="DR6" s="21">
         <f>SUMPRODUCT((DQ3:DQ8=DQ6)*(DN3:DN8&gt;DN6))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DS6" s="21">
         <f>SUMPRODUCT((DQ3:DQ8=DQ6)*(DN3:DN8=DN6)*(DL3:DL8&gt;DL6))</f>
@@ -11466,7 +11466,7 @@
       </c>
       <c r="DU6" s="21">
         <f t="shared" si="1"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="DV6" s="21" t="s">
         <v>39</v>
@@ -11604,7 +11604,7 @@
       <c r="IU6" s="21"/>
       <c r="IV6" s="21"/>
     </row>
-    <row r="7" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A7" s="21">
         <f>VLOOKUP(B7,CW4:CX8,2,FALSE)</f>
         <v>4</v>
@@ -11619,11 +11619,11 @@
       </c>
       <c r="D7" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B7)*(DD3:DD42="D"))+SUMPRODUCT((DC3:DC42=B7)*(DE3:DE42="D"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B7)*(DD3:DD42="L"))+SUMPRODUCT((DC3:DC42=B7)*(DE3:DE42="L"))</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F7" s="21">
         <f>SUMIF(CZ3:CZ60,B7,DA3:DA60)+SUMIF(DC3:DC60,B7,DB3:DB60)</f>
@@ -11631,15 +11631,15 @@
       </c>
       <c r="G7" s="21">
         <f>SUMIF(DC3:DC60,B7,DA3:DA60)+SUMIF(CZ3:CZ60,B7,DB3:DB60)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="H7" s="21">
         <f t="shared" si="2"/>
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="I7" s="21">
         <f t="shared" si="3"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7" s="21">
         <v>47</v>
@@ -12220,7 +12220,7 @@
       <c r="IU7" s="21"/>
       <c r="IV7" s="21"/>
     </row>
-    <row r="8" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A8" s="21"/>
       <c r="B8" s="21"/>
       <c r="C8" s="21"/>
@@ -12544,7 +12544,7 @@
       <c r="IU8" s="21"/>
       <c r="IV8" s="21"/>
     </row>
-    <row r="9" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A9" s="21"/>
       <c r="B9" s="21"/>
       <c r="C9" s="21"/>
@@ -12824,7 +12824,7 @@
       <c r="IU9" s="21"/>
       <c r="IV9" s="21"/>
     </row>
-    <row r="10" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A10" s="21"/>
       <c r="B10" s="21"/>
       <c r="C10" s="21"/>
@@ -13102,7 +13102,7 @@
       <c r="IU10" s="21"/>
       <c r="IV10" s="21"/>
     </row>
-    <row r="11" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A11" s="21">
         <f>VLOOKUP(B11,CW11:CX15,2,FALSE)</f>
         <v>1</v>
@@ -13498,7 +13498,7 @@
       <c r="IU11" s="21"/>
       <c r="IV11" s="21"/>
     </row>
-    <row r="12" spans="1:256" ht="13.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:256" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="21">
         <f>VLOOKUP(B12,CW11:CX15,2,FALSE)</f>
         <v>3</v>
@@ -13833,7 +13833,7 @@
       </c>
       <c r="DR12" s="199" t="str">
         <f>Matches!AC44</f>
-        <v>C</v>
+        <v>A</v>
       </c>
       <c r="DS12" s="199" t="str">
         <f>Matches!AC45</f>
@@ -13976,7 +13976,7 @@
       <c r="IU12" s="198"/>
       <c r="IV12" s="198"/>
     </row>
-    <row r="13" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A13" s="21">
         <f>IF(IW21=0,VLOOKUP(B13,CW11:CX15,2,FALSE),1)</f>
         <v>2</v>
@@ -14374,7 +14374,7 @@
       </c>
       <c r="DR13" s="199">
         <f>IFERROR(MATCH(DR12,DH13:DK13,0),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="DS13" s="199">
         <f>IFERROR(MATCH(DS12,DH13:DK13,0),0)</f>
@@ -14386,7 +14386,7 @@
       </c>
       <c r="DU13" s="199">
         <f t="shared" ref="DU13:DU27" si="22">SUM(DQ13:DT13)</f>
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="DV13" s="198"/>
       <c r="DW13" s="198" t="str">
@@ -14523,7 +14523,7 @@
       <c r="IU13" s="198"/>
       <c r="IV13" s="198"/>
     </row>
-    <row r="14" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A14" s="21">
         <f>VLOOKUP(B14,CW11:CX15,2,FALSE)</f>
         <v>4</v>
@@ -14978,7 +14978,7 @@
       </c>
       <c r="DR14" s="199">
         <f>IFERROR(MATCH(DR12,DH14:DK14,0),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="DS14" s="199">
         <f>IFERROR(MATCH(DS12,DH14:DK14,0),0)</f>
@@ -14990,12 +14990,12 @@
       </c>
       <c r="DU14" s="199">
         <f t="shared" si="22"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="DV14" s="198"/>
       <c r="DW14" s="198" t="str">
         <f>INDEX(DH3:DH8,MATCH(2,DU3:DU8,0),0)</f>
-        <v>Austria</v>
+        <v>Turkey</v>
       </c>
       <c r="DX14" s="198"/>
       <c r="DY14" s="21"/>
@@ -15127,7 +15127,7 @@
       <c r="IU14" s="198"/>
       <c r="IV14" s="198"/>
     </row>
-    <row r="15" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A15" s="21"/>
       <c r="B15" s="21"/>
       <c r="C15" s="21"/>
@@ -15290,7 +15290,7 @@
       </c>
       <c r="DR15" s="199">
         <f>IFERROR(MATCH(DR12,DH15:DK15,0),0)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="DS15" s="199">
         <f>IFERROR(MATCH(DS12,DH15:DK15,0),0)</f>
@@ -15302,7 +15302,7 @@
       </c>
       <c r="DU15" s="199">
         <f t="shared" si="22"/>
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="DV15" s="198"/>
       <c r="DW15" s="198" t="str">
@@ -15439,7 +15439,7 @@
       <c r="IU15" s="198"/>
       <c r="IV15" s="198"/>
     </row>
-    <row r="16" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A16" s="21"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -15604,7 +15604,7 @@
       </c>
       <c r="DR16" s="199">
         <f>IFERROR(MATCH(DR12,DH16:DK16,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DS16" s="199">
         <f>IFERROR(MATCH(DS12,DH16:DK16,0),0)</f>
@@ -15616,7 +15616,7 @@
       </c>
       <c r="DU16" s="199">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="DV16" s="198"/>
       <c r="DW16" s="198" t="str">
@@ -15753,7 +15753,7 @@
       <c r="IU16" s="198"/>
       <c r="IV16" s="198"/>
     </row>
-    <row r="17" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A17" s="21"/>
       <c r="B17" s="21"/>
       <c r="C17" s="21"/>
@@ -15916,7 +15916,7 @@
       </c>
       <c r="DR17" s="199">
         <f>IFERROR(MATCH(DR12,DH17:DK17,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DS17" s="199">
         <f>IFERROR(MATCH(DS12,DH17:DK17,0),0)</f>
@@ -15928,7 +15928,7 @@
       </c>
       <c r="DU17" s="199">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="DV17" s="198"/>
       <c r="DW17" s="198"/>
@@ -16062,7 +16062,7 @@
       <c r="IU17" s="198"/>
       <c r="IV17" s="198"/>
     </row>
-    <row r="18" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A18" s="21">
         <f>VLOOKUP(B18,CW18:CX22,2,FALSE)</f>
         <v>1</v>
@@ -16125,7 +16125,7 @@
       </c>
       <c r="Q18" s="21" t="str">
         <f>IF(O20=2,N19,"")</f>
-        <v>Austria</v>
+        <v/>
       </c>
       <c r="R18" s="21" t="str">
         <f>IF(O21=3,N20,"")</f>
@@ -16343,7 +16343,7 @@
       </c>
       <c r="DR18" s="199">
         <f>IFERROR(MATCH(DR12,DH18:DK18,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DS18" s="199">
         <f>IFERROR(MATCH(DS12,DH18:DK18,0),0)</f>
@@ -16355,14 +16355,14 @@
       </c>
       <c r="DU18" s="199">
         <f t="shared" si="22"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="DV18" s="198" t="s">
         <v>90</v>
       </c>
       <c r="DW18" s="198" t="str">
         <f>INDEX(DH3:DH8,MATCH(INDEX(DL13:DL27,MATCH(10,DU13:DU27,0),0),DV3:DV8,0),0)</f>
-        <v>Portugal</v>
+        <v>Sweden</v>
       </c>
       <c r="DX18" s="198"/>
       <c r="DY18" s="21"/>
@@ -16494,7 +16494,7 @@
       <c r="IU18" s="198"/>
       <c r="IV18" s="198"/>
     </row>
-    <row r="19" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A19" s="21">
         <f>VLOOKUP(B19,CW18:CX22,2,FALSE)</f>
         <v>2</v>
@@ -16505,11 +16505,11 @@
       </c>
       <c r="C19" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B19)*(DD3:DD42="W"))+SUMPRODUCT((DC3:DC42=B19)*(DE3:DE42="W"))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B19)*(DD3:DD42="D"))+SUMPRODUCT((DC3:DC42=B19)*(DE3:DE42="D"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E19" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B19)*(DD3:DD42="L"))+SUMPRODUCT((DC3:DC42=B19)*(DE3:DE42="L"))</f>
@@ -16517,7 +16517,7 @@
       </c>
       <c r="F19" s="21">
         <f>SUMIF(CZ3:CZ60,B19,DA3:DA60)+SUMIF(DC3:DC60,B19,DB3:DB60)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G19" s="21">
         <f>SUMIF(DC3:DC60,B19,DA3:DA60)+SUMIF(CZ3:CZ60,B19,DB3:DB60)</f>
@@ -16525,11 +16525,11 @@
       </c>
       <c r="H19" s="21">
         <f t="shared" si="25"/>
-        <v>1000</v>
+        <v>1001</v>
       </c>
       <c r="I19" s="21">
         <f t="shared" si="26"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J19" s="21">
         <v>50</v>
@@ -16541,11 +16541,11 @@
       <c r="L19" s="21"/>
       <c r="M19" s="21">
         <f>SUMPRODUCT((K18:K21=K19)*(J18:J21&lt;J19))+K19</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N19" s="21" t="str">
         <f>INDEX(B18:B22,MATCH(2,M18:M22,0),0)</f>
-        <v>Austria</v>
+        <v>Ukraine</v>
       </c>
       <c r="O19" s="21">
         <f>INDEX(K18:K22,MATCH(N19,B18:B22,0),0)</f>
@@ -16557,7 +16557,7 @@
       </c>
       <c r="Q19" s="21" t="str">
         <f>IF(Q18&lt;&gt;"",N20,"")</f>
-        <v>Ukraine</v>
+        <v/>
       </c>
       <c r="R19" s="21" t="str">
         <f>IF(R18&lt;&gt;"",N21,"")</f>
@@ -16650,7 +16650,7 @@
       </c>
       <c r="AO19" s="21" t="str">
         <f>IF(Q18&lt;&gt;"",Q18,"")</f>
-        <v>Austria</v>
+        <v/>
       </c>
       <c r="AP19" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO20)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO21)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO22)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO19)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO21)*(DC3:DC42=AO19)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO22)*(DC3:DC42=AO19)*(DE3:DE42="W"))</f>
@@ -16658,7 +16658,7 @@
       </c>
       <c r="AQ19" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO20)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO21)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO22)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO19)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO21)*(DC3:DC42=AO19)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO22)*(DC3:DC42=AO19)*(DD3:DD42="D"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR19" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO20)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO21)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO22)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO19)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO21)*(DC3:DC42=AO19)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO22)*(DC3:DC42=AO19)*(DE3:DE42="L"))</f>
@@ -16676,57 +16676,57 @@
         <f>AS19-AT19+1000</f>
         <v>1000</v>
       </c>
-      <c r="AV19" s="21">
+      <c r="AV19" s="21" t="str">
         <f t="shared" ref="AV19:AV21" si="30">IF(AO19&lt;&gt;"",AP19*3+AQ19*1,"")</f>
-        <v>1</v>
-      </c>
-      <c r="AW19" s="21">
+        <v/>
+      </c>
+      <c r="AW19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",VLOOKUP(AO19,B4:H40,7,FALSE),"")</f>
-        <v>1000</v>
-      </c>
-      <c r="AX19" s="21">
+        <v/>
+      </c>
+      <c r="AX19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",VLOOKUP(AO19,B4:H40,5,FALSE),"")</f>
-        <v>1</v>
-      </c>
-      <c r="AY19" s="21">
+        <v/>
+      </c>
+      <c r="AY19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",VLOOKUP(AO19,B4:J40,9,FALSE),"")</f>
-        <v>40</v>
-      </c>
-      <c r="AZ19" s="21">
+        <v/>
+      </c>
+      <c r="AZ19" s="21" t="str">
         <f t="shared" ref="AZ19:AZ21" si="31">AV19</f>
-        <v>1</v>
-      </c>
-      <c r="BA19" s="21">
+        <v/>
+      </c>
+      <c r="BA19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",RANK(AZ19,AZ18:AZ22),"")</f>
-        <v>1</v>
-      </c>
-      <c r="BB19" s="21">
+        <v/>
+      </c>
+      <c r="BB19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ19)*(AU18:AU22&gt;AU19)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BC19" s="21">
+        <v/>
+      </c>
+      <c r="BC19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ19)*(AU18:AU22=AU19)*(AS18:AS22&gt;AS19)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BD19" s="21">
+        <v/>
+      </c>
+      <c r="BD19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ19)*(AU18:AU22=AU19)*(AS18:AS22=AS19)*(AW18:AW22&gt;AW19)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BE19" s="21">
+        <v/>
+      </c>
+      <c r="BE19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ19)*(AU18:AU22=AU19)*(AS18:AS22=AS19)*(AW18:AW22=AW19)*(AX18:AX22&gt;AX19)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="BF19" s="21">
+        <v/>
+      </c>
+      <c r="BF19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ19)*(AU18:AU22=AU19)*(AS18:AS22=AS19)*(AW18:AW22=AW19)*(AX18:AX22=AX19)*(AY18:AY22&gt;AY19)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BG19" s="21">
+        <v/>
+      </c>
+      <c r="BG19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",IF(BG59&lt;&gt;"",IF(AN57=3,BG59,BG59+AN57),SUM(BA19:BF19)+1),"")</f>
-        <v>3</v>
+        <v/>
       </c>
       <c r="BH19" s="21" t="str">
         <f>IF(AO19&lt;&gt;"",INDEX(AO19:AO22,MATCH(2,BG19:BG22,0),0),"")</f>
-        <v>Ukraine</v>
+        <v/>
       </c>
       <c r="BI19" s="21"/>
       <c r="BJ19" s="21"/>
@@ -16835,7 +16835,7 @@
       </c>
       <c r="DR19" s="199">
         <f>IFERROR(MATCH(DR12,DH19:DK19,0),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DS19" s="199">
         <f>IFERROR(MATCH(DS12,DH19:DK19,0),0)</f>
@@ -16847,14 +16847,14 @@
       </c>
       <c r="DU19" s="199">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="DV19" s="198" t="s">
         <v>85</v>
       </c>
       <c r="DW19" s="198" t="str">
         <f>INDEX(DH3:DH8,MATCH(INDEX(DM13:DM27,MATCH(10,DU13:DU27,0),0),DV3:DV8,0),0)</f>
-        <v>Sweden</v>
+        <v>Portugal</v>
       </c>
       <c r="DX19" s="198"/>
       <c r="DY19" s="21"/>
@@ -16986,7 +16986,7 @@
       <c r="IU19" s="198"/>
       <c r="IV19" s="198"/>
     </row>
-    <row r="20" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A20" s="21">
         <f>VLOOKUP(B20,CW18:CX22,2,FALSE)</f>
         <v>3</v>
@@ -17001,11 +17001,11 @@
       </c>
       <c r="D20" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B20)*(DD3:DD42="D"))+SUMPRODUCT((DC3:DC42=B20)*(DE3:DE42="D"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=B20)*(DD3:DD42="L"))+SUMPRODUCT((DC3:DC42=B20)*(DE3:DE42="L"))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F20" s="21">
         <f>SUMIF(CZ3:CZ60,B20,DA3:DA60)+SUMIF(DC3:DC60,B20,DB3:DB60)</f>
@@ -17013,35 +17013,35 @@
       </c>
       <c r="G20" s="21">
         <f>SUMIF(DC3:DC60,B20,DA3:DA60)+SUMIF(CZ3:CZ60,B20,DB3:DB60)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H20" s="21">
         <f t="shared" si="25"/>
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="I20" s="21">
         <f t="shared" si="26"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J20" s="21">
         <v>40</v>
       </c>
       <c r="K20" s="21">
         <f>IF(COUNTIF(I18:I22,4)&lt;&gt;4,RANK(I20,I18:I22),I60)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L20" s="21"/>
       <c r="M20" s="21">
         <f>SUMPRODUCT((K18:K21=K20)*(J18:J21&lt;J20))+K20</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="N20" s="21" t="str">
         <f>INDEX(B18:B22,MATCH(3,M18:M22,0),0)</f>
-        <v>Ukraine</v>
+        <v>Austria</v>
       </c>
       <c r="O20" s="21">
         <f>INDEX(K18:K22,MATCH(N20,B18:B22,0),0)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P20" s="21" t="str">
         <f>IF(AND(P19&lt;&gt;"",O20=1),N20,"")</f>
@@ -17139,7 +17139,7 @@
       </c>
       <c r="AO20" s="21" t="str">
         <f>IF(Q19&lt;&gt;"",Q19,"")</f>
-        <v>Ukraine</v>
+        <v/>
       </c>
       <c r="AP20" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO21)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO22)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO19)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO21)*(DC3:DC42=AO20)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO22)*(DC3:DC42=AO20)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO20)*(DE3:DE42="W"))</f>
@@ -17147,7 +17147,7 @@
       </c>
       <c r="AQ20" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO21)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO22)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO19)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO21)*(DC3:DC42=AO20)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO22)*(DC3:DC42=AO20)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO20)*(DD3:DD42="D"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR20" s="21">
         <f>SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO21)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO22)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO20)*(DC3:DC42=AO19)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO21)*(DC3:DC42=AO20)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO22)*(DC3:DC42=AO20)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO19)*(DC3:DC42=AO20)*(DE3:DE42="L"))</f>
@@ -17165,57 +17165,57 @@
         <f>AS20-AT20+1000</f>
         <v>1000</v>
       </c>
-      <c r="AV20" s="21">
+      <c r="AV20" s="21" t="str">
         <f t="shared" si="30"/>
-        <v>1</v>
-      </c>
-      <c r="AW20" s="21">
+        <v/>
+      </c>
+      <c r="AW20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",VLOOKUP(AO20,B4:H40,7,FALSE),"")</f>
-        <v>1000</v>
-      </c>
-      <c r="AX20" s="21">
+        <v/>
+      </c>
+      <c r="AX20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",VLOOKUP(AO20,B4:H40,5,FALSE),"")</f>
-        <v>2</v>
-      </c>
-      <c r="AY20" s="21">
+        <v/>
+      </c>
+      <c r="AY20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",VLOOKUP(AO20,B4:J40,9,FALSE),"")</f>
-        <v>50</v>
-      </c>
-      <c r="AZ20" s="21">
+        <v/>
+      </c>
+      <c r="AZ20" s="21" t="str">
         <f t="shared" si="31"/>
-        <v>1</v>
-      </c>
-      <c r="BA20" s="21">
+        <v/>
+      </c>
+      <c r="BA20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",RANK(AZ20,AZ18:AZ22),"")</f>
-        <v>1</v>
-      </c>
-      <c r="BB20" s="21">
+        <v/>
+      </c>
+      <c r="BB20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ20)*(AU18:AU22&gt;AU20)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BC20" s="21">
+        <v/>
+      </c>
+      <c r="BC20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ20)*(AU18:AU22=AU20)*(AS18:AS22&gt;AS20)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BD20" s="21">
+        <v/>
+      </c>
+      <c r="BD20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ20)*(AU18:AU22=AU20)*(AS18:AS22=AS20)*(AW18:AW22&gt;AW20)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BE20" s="21">
+        <v/>
+      </c>
+      <c r="BE20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ20)*(AU18:AU22=AU20)*(AS18:AS22=AS20)*(AW18:AW22=AW20)*(AX18:AX22&gt;AX20)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BF20" s="21">
+        <v/>
+      </c>
+      <c r="BF20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",SUMPRODUCT((AZ18:AZ22=AZ20)*(AU18:AU22=AU20)*(AS18:AS22=AS20)*(AW18:AW22=AW20)*(AX18:AX22=AX20)*(AY18:AY22&gt;AY20)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BG20" s="21">
+        <v/>
+      </c>
+      <c r="BG20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",IF(BG60&lt;&gt;"",IF(AN57=3,BG60,BG60+AN57),SUM(BA20:BF20)+1),"")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="BH20" s="21" t="str">
         <f>IF(AO20&lt;&gt;"",INDEX(AO19:AO22,MATCH(3,BG19:BG22,0),0),"")</f>
-        <v>Austria</v>
+        <v/>
       </c>
       <c r="BI20" s="21" t="str">
         <f>IF(R18&lt;&gt;"",R18,"")</f>
@@ -17384,7 +17384,7 @@
       </c>
       <c r="DR20" s="199">
         <f>IFERROR(MATCH(DR12,DH20:DK20,0),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DS20" s="199">
         <f>IFERROR(MATCH(DS12,DH20:DK20,0),0)</f>
@@ -17396,14 +17396,14 @@
       </c>
       <c r="DU20" s="199">
         <f t="shared" si="22"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="DV20" s="198" t="s">
         <v>86</v>
       </c>
       <c r="DW20" s="198" t="str">
         <f>INDEX(DH3:DH8,MATCH(INDEX(DN13:DN27,MATCH(10,DU13:DU27,0),0),DV3:DV8,0),0)</f>
-        <v>Austria</v>
+        <v>Russia</v>
       </c>
       <c r="DX20" s="198"/>
       <c r="DY20" s="21"/>
@@ -17535,7 +17535,7 @@
       <c r="IU20" s="198"/>
       <c r="IV20" s="198"/>
     </row>
-    <row r="21" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A21" s="21">
         <f>VLOOKUP(B21,CW18:CX22,2,FALSE)</f>
         <v>4</v>
@@ -17990,7 +17990,7 @@
       </c>
       <c r="DR21" s="199">
         <f>IFERROR(MATCH(DR12,DH21:DK21,0),0)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="DS21" s="199">
         <f>IFERROR(MATCH(DS12,DH21:DK21,0),0)</f>
@@ -18002,14 +18002,14 @@
       </c>
       <c r="DU21" s="199">
         <f t="shared" si="22"/>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="DV21" s="198" t="s">
         <v>91</v>
       </c>
       <c r="DW21" s="198" t="str">
         <f>INDEX(DH3:DH8,MATCH(INDEX(DO13:DO27,MATCH(10,DU13:DU27,0),0),DV3:DV8,0),0)</f>
-        <v>Russia</v>
+        <v>Turkey</v>
       </c>
       <c r="DX21" s="198"/>
       <c r="DY21" s="21"/>
@@ -18141,7 +18141,7 @@
       <c r="IU21" s="198"/>
       <c r="IV21" s="198"/>
     </row>
-    <row r="22" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A22" s="21"/>
       <c r="B22" s="21"/>
       <c r="C22" s="21"/>
@@ -18304,7 +18304,7 @@
       </c>
       <c r="DR22" s="199">
         <f>IFERROR(MATCH(DR12,DH22:DK22,0),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DS22" s="199">
         <f>IFERROR(MATCH(DS12,DH22:DK22,0),0)</f>
@@ -18316,7 +18316,7 @@
       </c>
       <c r="DU22" s="199">
         <f t="shared" si="22"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="DV22" s="198" t="s">
         <v>42</v>
@@ -18455,7 +18455,7 @@
       <c r="IU22" s="198"/>
       <c r="IV22" s="198"/>
     </row>
-    <row r="23" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A23" s="21"/>
       <c r="B23" s="21"/>
       <c r="C23" s="21"/>
@@ -18618,7 +18618,7 @@
       </c>
       <c r="DR23" s="199">
         <f>IFERROR(MATCH(DR12,DH23:DK23,0),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DS23" s="199">
         <f>IFERROR(MATCH(DS12,DH23:DK23,0),0)</f>
@@ -18630,7 +18630,7 @@
       </c>
       <c r="DU23" s="199">
         <f t="shared" si="22"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="DV23" s="198"/>
       <c r="DW23" s="198" t="str">
@@ -18767,7 +18767,7 @@
       <c r="IU23" s="198"/>
       <c r="IV23" s="198"/>
     </row>
-    <row r="24" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A24" s="21"/>
       <c r="B24" s="21"/>
       <c r="C24" s="21"/>
@@ -18930,7 +18930,7 @@
       </c>
       <c r="DR24" s="199">
         <f>IFERROR(MATCH(DR12,DH24:DK24,0),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DS24" s="199">
         <f>IFERROR(MATCH(DS12,DH24:DK24,0),0)</f>
@@ -18942,7 +18942,7 @@
       </c>
       <c r="DU24" s="199">
         <f t="shared" si="22"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="DV24" s="198" t="s">
         <v>46</v>
@@ -19081,7 +19081,7 @@
       <c r="IU24" s="198"/>
       <c r="IV24" s="198"/>
     </row>
-    <row r="25" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A25" s="21">
         <f>VLOOKUP(B25,CW25:CX29,2,FALSE)</f>
         <v>3</v>
@@ -19362,7 +19362,7 @@
       </c>
       <c r="DR25" s="199">
         <f>IFERROR(MATCH(DR12,DH25:DK25,0),0)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="DS25" s="199">
         <f>IFERROR(MATCH(DS12,DH25:DK25,0),0)</f>
@@ -19374,7 +19374,7 @@
       </c>
       <c r="DU25" s="199">
         <f t="shared" si="22"/>
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="DV25" s="198"/>
       <c r="DW25" s="198" t="str">
@@ -19511,7 +19511,7 @@
       <c r="IU25" s="198"/>
       <c r="IV25" s="198"/>
     </row>
-    <row r="26" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A26" s="21">
         <f>VLOOKUP(B26,CW25:CX29,2,FALSE)</f>
         <v>4</v>
@@ -20003,7 +20003,7 @@
       <c r="IU26" s="198"/>
       <c r="IV26" s="198"/>
     </row>
-    <row r="27" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A27" s="21">
         <f>VLOOKUP(B27,CW25:CX29,2,FALSE)</f>
         <v>1</v>
@@ -20354,7 +20354,7 @@
       </c>
       <c r="DB27" s="21">
         <f>IF(AND(Matches!G35&lt;&gt;"",Matches!F35&lt;&gt;""),Matches!G35,0)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="DC27" s="21" t="str">
         <f>Matches!H35</f>
@@ -20362,11 +20362,11 @@
       </c>
       <c r="DD27" s="21" t="str">
         <f>IF(AND(Matches!F35&lt;&gt;"",Matches!G35&lt;&gt;""),IF(DA27&gt;DB27,"W",IF(DA27=DB27,"D","L")),"")</f>
-        <v>D</v>
+        <v>L</v>
       </c>
       <c r="DE27" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>D</v>
+        <v>W</v>
       </c>
       <c r="DF27" s="21"/>
       <c r="DG27" s="21"/>
@@ -20401,7 +20401,7 @@
       </c>
       <c r="DR27" s="199">
         <f>IFERROR(MATCH(DR12,DH27:DK27,0),0)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="DS27" s="199">
         <f>IFERROR(MATCH(DS12,DH27:DK27,0),0)</f>
@@ -20413,7 +20413,7 @@
       </c>
       <c r="DU27" s="199">
         <f t="shared" si="22"/>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="DV27" s="21"/>
       <c r="DW27" s="21" t="str">
@@ -20550,7 +20550,7 @@
       <c r="IU27" s="21"/>
       <c r="IV27" s="198"/>
     </row>
-    <row r="28" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A28" s="21">
         <f>VLOOKUP(B28,CW25:CX29,2,FALSE)</f>
         <v>2</v>
@@ -21125,7 +21125,7 @@
       <c r="IU28" s="21"/>
       <c r="IV28" s="198"/>
     </row>
-    <row r="29" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A29" s="21"/>
       <c r="B29" s="21"/>
       <c r="C29" s="21"/>
@@ -21409,7 +21409,7 @@
       <c r="IU29" s="21"/>
       <c r="IV29" s="198"/>
     </row>
-    <row r="30" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A30" s="21"/>
       <c r="B30" s="21"/>
       <c r="C30" s="21"/>
@@ -21526,7 +21526,7 @@
       </c>
       <c r="DA30" s="21">
         <f>IF(AND(Matches!F38&lt;&gt;"",Matches!G38&lt;&gt;""),Matches!F38,0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DB30" s="21">
         <f>IF(AND(Matches!G38&lt;&gt;"",Matches!F38&lt;&gt;""),Matches!G38,0)</f>
@@ -21538,11 +21538,11 @@
       </c>
       <c r="DD30" s="21" t="str">
         <f>IF(AND(Matches!F38&lt;&gt;"",Matches!G38&lt;&gt;""),IF(DA30&gt;DB30,"W",IF(DA30=DB30,"D","L")),"")</f>
-        <v>D</v>
+        <v>W</v>
       </c>
       <c r="DE30" s="21" t="str">
         <f t="shared" si="0"/>
-        <v>D</v>
+        <v>L</v>
       </c>
       <c r="DF30" s="21"/>
       <c r="DG30" s="21"/>
@@ -21697,7 +21697,7 @@
       <c r="IU30" s="21"/>
       <c r="IV30" s="198"/>
     </row>
-    <row r="31" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A31" s="21">
         <f>VLOOKUP(B31,CW31:CX35,2,FALSE)</f>
         <v>1</v>
@@ -22096,7 +22096,7 @@
       <c r="IU31" s="21"/>
       <c r="IV31" s="198"/>
     </row>
-    <row r="32" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A32" s="21">
         <f>VLOOKUP(B32,CW31:CX35,2,FALSE)</f>
         <v>3</v>
@@ -22557,7 +22557,7 @@
       <c r="IU32" s="21"/>
       <c r="IV32" s="198"/>
     </row>
-    <row r="33" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A33" s="21">
         <f>VLOOKUP(B33,CW31:CX35,2,FALSE)</f>
         <v>2</v>
@@ -23073,7 +23073,7 @@
       <c r="IU33" s="21"/>
       <c r="IV33" s="198"/>
     </row>
-    <row r="34" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A34" s="21">
         <f>VLOOKUP(B34,CW31:CX35,2,FALSE)</f>
         <v>4</v>
@@ -23643,7 +23643,7 @@
       <c r="IU34" s="21"/>
       <c r="IV34" s="21"/>
     </row>
-    <row r="35" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A35" s="21"/>
       <c r="B35" s="21"/>
       <c r="C35" s="21"/>
@@ -23921,7 +23921,7 @@
       <c r="IU35" s="21"/>
       <c r="IV35" s="21"/>
     </row>
-    <row r="36" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A36" s="21"/>
       <c r="B36" s="21"/>
       <c r="C36" s="21"/>
@@ -24199,7 +24199,7 @@
       <c r="IU36" s="21"/>
       <c r="IV36" s="21"/>
     </row>
-    <row r="37" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A37" s="21">
         <f>VLOOKUP(B37,CW37:CX41,2,FALSE)</f>
         <v>1</v>
@@ -24595,7 +24595,7 @@
       <c r="IU37" s="21"/>
       <c r="IV37" s="21"/>
     </row>
-    <row r="38" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A38" s="21">
         <f>VLOOKUP(B38,CW37:CX41,2,FALSE)</f>
         <v>2</v>
@@ -25051,7 +25051,7 @@
       <c r="IU38" s="21"/>
       <c r="IV38" s="21"/>
     </row>
-    <row r="39" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A39" s="21">
         <f>VLOOKUP(B39,CW37:CX41,2,FALSE)</f>
         <v>4</v>
@@ -25544,7 +25544,7 @@
       <c r="IU39" s="21"/>
       <c r="IV39" s="21"/>
     </row>
-    <row r="40" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A40" s="21">
         <f>VLOOKUP(B40,CW37:CX41,2,FALSE)</f>
         <v>3</v>
@@ -26094,7 +26094,7 @@
       <c r="IU40" s="21"/>
       <c r="IV40" s="21"/>
     </row>
-    <row r="41" spans="1:256" ht="14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:256" ht="13.8" x14ac:dyDescent="0.3">
       <c r="A41" s="21"/>
       <c r="B41" s="21"/>
       <c r="C41" s="21"/>
@@ -26352,12 +26352,12 @@
       <c r="IU41" s="21"/>
       <c r="IV41" s="21"/>
     </row>
-    <row r="42" spans="1:256" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:256" ht="11.55" customHeight="1" x14ac:dyDescent="0.2">
       <c r="DC42" s="194" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="43" spans="1:256" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:256" x14ac:dyDescent="0.2">
       <c r="T43" s="194">
         <f>IF(U44="",SUM(AG4:AL4),IF(U45="",SUM(AG5:AL5),IF(U46="",SUM(AG6:AL6),IF(U47="",SUM(AG7:AL7),0))))</f>
         <v>0</v>
@@ -26481,7 +26481,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="44" spans="1:256" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:256" x14ac:dyDescent="0.2">
       <c r="I44" s="194">
         <f>SUMPRODUCT((I4:I7=I4)*(H4:H7=H4)*(F4:F7&gt;F4))+1</f>
         <v>1</v>
@@ -26567,7 +26567,7 @@
         <v/>
       </c>
     </row>
-    <row r="45" spans="1:256" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:256" x14ac:dyDescent="0.2">
       <c r="I45" s="194">
         <f>SUMPRODUCT((I4:I7=I5)*(H4:H7=H5)*(F4:F7&gt;F5))+1</f>
         <v>1</v>
@@ -26733,7 +26733,7 @@
         <v/>
       </c>
     </row>
-    <row r="46" spans="1:256" x14ac:dyDescent="0.15">
+    <row r="46" spans="1:256" x14ac:dyDescent="0.2">
       <c r="I46" s="194">
         <f>SUMPRODUCT((I4:I7=I6)*(H4:H7=H6)*(F4:F7&gt;F6))+1</f>
         <v>1</v>
@@ -26899,7 +26899,7 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:256" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:256" x14ac:dyDescent="0.2">
       <c r="I47" s="194">
         <f>SUMPRODUCT((I4:I7=I7)*(H4:H7=H7)*(F4:F7&gt;F7))+1</f>
         <v>1</v>
@@ -27065,7 +27065,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="50" spans="2:59" x14ac:dyDescent="0.2">
       <c r="B50" s="194" t="str">
         <f>B4</f>
         <v>Turkey</v>
@@ -27082,7 +27082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="51" spans="2:59" x14ac:dyDescent="0.2">
       <c r="B51" s="194" t="str">
         <f t="shared" ref="B51:B53" si="76">B5</f>
         <v>Italy</v>
@@ -27175,7 +27175,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="52" spans="2:59" x14ac:dyDescent="0.2">
       <c r="B52" s="194" t="str">
         <f t="shared" si="76"/>
         <v>Wales</v>
@@ -27348,7 +27348,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="53" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="53" spans="2:59" x14ac:dyDescent="0.2">
       <c r="B53" s="194" t="str">
         <f t="shared" si="76"/>
         <v>Switzerland</v>
@@ -27521,7 +27521,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="54" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="54" spans="2:59" x14ac:dyDescent="0.2">
       <c r="C54" s="194" t="s">
         <v>100</v>
       </c>
@@ -27690,17 +27690,17 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="55" spans="2:59" x14ac:dyDescent="0.2">
       <c r="C55" s="194" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="56" spans="2:59" x14ac:dyDescent="0.2">
       <c r="C56" s="194" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="57" spans="2:59" x14ac:dyDescent="0.2">
       <c r="C57" s="194" t="s">
         <v>103</v>
       </c>
@@ -27713,7 +27713,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="58" spans="2:59" x14ac:dyDescent="0.2">
       <c r="C58" s="194" t="s">
         <v>104</v>
       </c>
@@ -27802,7 +27802,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="59" spans="2:59" x14ac:dyDescent="0.2">
       <c r="C59" s="194" t="s">
         <v>105</v>
       </c>
@@ -27890,13 +27890,13 @@
         <f>IF(U59&lt;&gt;"",SUM(AG59:AL59),"")</f>
         <v/>
       </c>
-      <c r="AN59" s="194">
+      <c r="AN59" s="194" t="str">
         <f>IF(AO19&lt;&gt;"",SUMPRODUCT((AV18:AV21=AV19)*(AU18:AU21=AU19)*(AS18:AS21=AS19)*(AT18:AT21=AT19)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AO59" s="194" t="str">
         <f t="shared" ref="AO59:AO61" si="88">IF(AND(AN59&lt;&gt;"",AN59&gt;1),AO19,"")</f>
-        <v>Austria</v>
+        <v/>
       </c>
       <c r="AP59" s="194">
         <f>SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO60)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO61)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO62)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO59)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO61)*(DC3:DC42=AO59)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO62)*(DC3:DC42=AO59)*(DE3:DE42="W"))</f>
@@ -27904,7 +27904,7 @@
       </c>
       <c r="AQ59" s="194">
         <f>SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO60)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO61)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO62)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO59)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO61)*(DC3:DC42=AO59)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO62)*(DC3:DC42=AO59)*(DD3:DD42="D"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR59" s="194">
         <f>SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO60)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO61)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO62)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO59)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO61)*(DC3:DC42=AO59)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO62)*(DC3:DC42=AO59)*(DE3:DE42="L"))</f>
@@ -27922,59 +27922,59 @@
         <f>AS59-AT59+1000</f>
         <v>1000</v>
       </c>
-      <c r="AV59" s="194">
+      <c r="AV59" s="194" t="str">
         <f t="shared" ref="AV59:AV61" si="89">IF(AO59&lt;&gt;"",AP59*3+AQ59*1,"")</f>
-        <v>1</v>
-      </c>
-      <c r="AW59" s="194">
+        <v/>
+      </c>
+      <c r="AW59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",VLOOKUP(AO59,B4:H40,7,FALSE),"")</f>
-        <v>1000</v>
-      </c>
-      <c r="AX59" s="194">
+        <v/>
+      </c>
+      <c r="AX59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",VLOOKUP(AO59,B4:H40,5,FALSE),"")</f>
-        <v>1</v>
-      </c>
-      <c r="AY59" s="194">
+        <v/>
+      </c>
+      <c r="AY59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",VLOOKUP(AO59,B4:J40,9,FALSE),"")</f>
-        <v>40</v>
-      </c>
-      <c r="AZ59" s="194">
+        <v/>
+      </c>
+      <c r="AZ59" s="194" t="str">
         <f t="shared" ref="AZ59:AZ61" si="90">AV59</f>
-        <v>1</v>
-      </c>
-      <c r="BA59" s="194">
+        <v/>
+      </c>
+      <c r="BA59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",RANK(AZ59,AZ58:AZ61),"")</f>
-        <v>1</v>
-      </c>
-      <c r="BB59" s="194">
+        <v/>
+      </c>
+      <c r="BB59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ59)*(AU58:AU61&gt;AU59)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BC59" s="194">
+        <v/>
+      </c>
+      <c r="BC59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ59)*(AU58:AU61=AU59)*(AS58:AS61&gt;AS59)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BD59" s="194">
+        <v/>
+      </c>
+      <c r="BD59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ59)*(AU58:AU61=AU59)*(AS58:AS61=AS59)*(AW58:AW61&gt;AW59)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BE59" s="194">
+        <v/>
+      </c>
+      <c r="BE59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ59)*(AU58:AU61=AU59)*(AS58:AS61=AS59)*(AW58:AW61=AW59)*(AX58:AX61&gt;AX59)),"")</f>
-        <v>1</v>
-      </c>
-      <c r="BF59" s="194">
+        <v/>
+      </c>
+      <c r="BF59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ59)*(AU58:AU61=AU59)*(AS58:AS61=AS59)*(AW58:AW61=AW59)*(AX58:AX61=AX59)*(AY58:AY61&gt;AY59)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BG59" s="194">
+        <v/>
+      </c>
+      <c r="BG59" s="194" t="str">
         <f>IF(AO59&lt;&gt;"",SUM(BA59:BF59)+1,"")</f>
-        <v>3</v>
+        <v/>
       </c>
     </row>
-    <row r="60" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="60" spans="2:59" x14ac:dyDescent="0.2">
       <c r="I60" s="194">
         <f>SUMPRODUCT((I18:I21=I20)*(H18:H21=H20)*(F18:F21&gt;F20))+1</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="T60" s="194" t="str">
         <f>IF(U20&lt;&gt;"",SUMPRODUCT((AB18:AB21=AB20)*(AA18:AA21=AA20)*(Y18:Y21=Y20)*(Z18:Z21=Z20)),"")</f>
@@ -28056,13 +28056,13 @@
         <f>IF(U60&lt;&gt;"",SUM(AG60:AL60),"")</f>
         <v/>
       </c>
-      <c r="AN60" s="194">
+      <c r="AN60" s="194" t="str">
         <f>IF(AO20&lt;&gt;"",SUMPRODUCT((AV18:AV21=AV20)*(AU18:AU21=AU20)*(AS18:AS21=AS20)*(AT18:AT21=AT20)),"")</f>
-        <v>2</v>
+        <v/>
       </c>
       <c r="AO60" s="194" t="str">
         <f t="shared" si="88"/>
-        <v>Ukraine</v>
+        <v/>
       </c>
       <c r="AP60" s="194">
         <f>SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO61)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO62)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO59)*(DD3:DD42="W"))+SUMPRODUCT((CZ3:CZ42=AO61)*(DC3:DC42=AO60)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO62)*(DC3:DC42=AO60)*(DE3:DE42="W"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO60)*(DE3:DE42="W"))</f>
@@ -28070,7 +28070,7 @@
       </c>
       <c r="AQ60" s="194">
         <f>SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO61)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO62)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO59)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO61)*(DC3:DC42=AO60)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO62)*(DC3:DC42=AO60)*(DD3:DD42="D"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO60)*(DD3:DD42="D"))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR60" s="194">
         <f>SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO61)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO62)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO60)*(DC3:DC42=AO59)*(DD3:DD42="L"))+SUMPRODUCT((CZ3:CZ42=AO61)*(DC3:DC42=AO60)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO62)*(DC3:DC42=AO60)*(DE3:DE42="L"))+SUMPRODUCT((CZ3:CZ42=AO59)*(DC3:DC42=AO60)*(DE3:DE42="L"))</f>
@@ -28088,56 +28088,56 @@
         <f>AS60-AT60+1000</f>
         <v>1000</v>
       </c>
-      <c r="AV60" s="194">
+      <c r="AV60" s="194" t="str">
         <f t="shared" si="89"/>
-        <v>1</v>
-      </c>
-      <c r="AW60" s="194">
+        <v/>
+      </c>
+      <c r="AW60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",VLOOKUP(AO60,B4:H40,7,FALSE),"")</f>
-        <v>1000</v>
-      </c>
-      <c r="AX60" s="194">
+        <v/>
+      </c>
+      <c r="AX60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",VLOOKUP(AO60,B4:H40,5,FALSE),"")</f>
-        <v>2</v>
-      </c>
-      <c r="AY60" s="194">
+        <v/>
+      </c>
+      <c r="AY60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",VLOOKUP(AO60,B4:J40,9,FALSE),"")</f>
-        <v>50</v>
-      </c>
-      <c r="AZ60" s="194">
+        <v/>
+      </c>
+      <c r="AZ60" s="194" t="str">
         <f t="shared" si="90"/>
-        <v>1</v>
-      </c>
-      <c r="BA60" s="194">
+        <v/>
+      </c>
+      <c r="BA60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",RANK(AZ60,AZ58:AZ61),"")</f>
-        <v>1</v>
-      </c>
-      <c r="BB60" s="194">
+        <v/>
+      </c>
+      <c r="BB60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ60)*(AU58:AU61&gt;AU60)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BC60" s="194">
+        <v/>
+      </c>
+      <c r="BC60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ60)*(AU58:AU61=AU60)*(AS58:AS61&gt;AS60)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BD60" s="194">
+        <v/>
+      </c>
+      <c r="BD60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ60)*(AU58:AU61=AU60)*(AS58:AS61=AS60)*(AW58:AW61&gt;AW60)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BE60" s="194">
+        <v/>
+      </c>
+      <c r="BE60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ60)*(AU58:AU61=AU60)*(AS58:AS61=AS60)*(AW58:AW61=AW60)*(AX58:AX61&gt;AX60)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BF60" s="194">
+        <v/>
+      </c>
+      <c r="BF60" s="194" t="str">
         <f>IF(AO60&lt;&gt;"",SUMPRODUCT((AZ58:AZ61=AZ60)*(AU58:AU61=AU60)*(AS58:AS61=AS60)*(AW58:AW61=AW60)*(AX58:AX61=AX60)*(AY58:AY61&gt;AY60)),"")</f>
-        <v>0</v>
-      </c>
-      <c r="BG60" s="194">
+        <v/>
+      </c>
+      <c r="BG60" s="194" t="str">
         <f t="shared" ref="BG60:BG61" si="91">IF(AO60&lt;&gt;"",SUM(BA60:BF60)+1,"")</f>
-        <v>2</v>
+        <v/>
       </c>
     </row>
-    <row r="61" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="61" spans="2:59" x14ac:dyDescent="0.2">
       <c r="I61" s="194">
         <f>SUMPRODUCT((I18:I21=I21)*(H18:H21=H21)*(F18:F21&gt;F21))+1</f>
         <v>1</v>
@@ -28303,7 +28303,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="2:59" x14ac:dyDescent="0.15">
+    <row r="64" spans="2:59" x14ac:dyDescent="0.2">
       <c r="T64" s="194">
         <f>IF(U65="",SUM(AG25:AL25),IF(U66="",SUM(AG26:AL26),IF(U67="",SUM(AG27:AL27),IF(U68="",SUM(AG28:AL28),0))))</f>
         <v>0</v>
@@ -28313,7 +28313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="65" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I65" s="194">
         <f>SUMPRODUCT((I25:I28=I25)*(H25:H28=H25)*(F25:F28&gt;F25))+1</f>
         <v>1</v>
@@ -28399,7 +28399,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="66" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="66" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I66" s="194">
         <f>SUMPRODUCT((I25:I28=I26)*(H25:H28=H26)*(F25:F28&gt;F26))+1</f>
         <v>1</v>
@@ -28565,7 +28565,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="67" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I67" s="194">
         <f>SUMPRODUCT((I25:I28=I27)*(H25:H28=H27)*(F25:F28&gt;F27))+1</f>
         <v>1</v>
@@ -28731,7 +28731,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="68" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I68" s="194">
         <f>SUMPRODUCT((I25:I28=I28)*(H25:H28=H28)*(F25:F28&gt;F28))+1</f>
         <v>1</v>
@@ -28897,7 +28897,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="70" spans="9:59" x14ac:dyDescent="0.2">
       <c r="T70" s="194">
         <f>IF(U71="",SUM(AG31:AL31),IF(U72="",SUM(AG32:AL32),IF(U73="",SUM(AG33:AL33),IF(U74="",SUM(AG34:AL34),0))))</f>
         <v>0</v>
@@ -28907,7 +28907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="71" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I71" s="194">
         <f>SUMPRODUCT((I31:I34=I31)*(H31:H34=H31)*(F31:F34&gt;F31))+1</f>
         <v>1</v>
@@ -28993,7 +28993,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="72" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I72" s="194">
         <f>SUMPRODUCT((I31:I34=I32)*(H31:H34=H32)*(F31:F34&gt;F32))+1</f>
         <v>1</v>
@@ -29159,7 +29159,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="73" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="73" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I73" s="194">
         <f>SUMPRODUCT((I31:I34=I33)*(H31:H34=H33)*(F31:F34&gt;F33))+1</f>
         <v>1</v>
@@ -29325,7 +29325,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="74" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="74" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I74" s="194">
         <f>SUMPRODUCT((I31:I34=I34)*(H31:H34=H34)*(F31:F34&gt;F34))+1</f>
         <v>1</v>
@@ -29491,7 +29491,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="76" spans="9:59" x14ac:dyDescent="0.2">
       <c r="T76" s="194">
         <f>IF(U77="",SUM(AG37:AL37),IF(U78="",SUM(AG38:AL38),IF(U79="",SUM(AG39:AL39),IF(U80="",SUM(AG40:AL40),0))))</f>
         <v>0</v>
@@ -29501,7 +29501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="77" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I77" s="194">
         <f>SUMPRODUCT((I37:I40=I37)*(H37:H40=H37)*(F37:F40&gt;F37))+1</f>
         <v>1</v>
@@ -29587,7 +29587,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="78" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I78" s="194">
         <f>SUMPRODUCT((I37:I40=I38)*(H37:H40=H38)*(F37:F40&gt;F38))+1</f>
         <v>1</v>
@@ -29753,7 +29753,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="79" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="79" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I79" s="194">
         <f>SUMPRODUCT((I37:I40=I39)*(H37:H40=H39)*(F37:F40&gt;F39))+1</f>
         <v>1</v>
@@ -29919,7 +29919,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="80" spans="9:59" x14ac:dyDescent="0.15">
+    <row r="80" spans="9:59" x14ac:dyDescent="0.2">
       <c r="I80" s="194">
         <f>SUMPRODUCT((I37:I40=I40)*(H37:H40=H40)*(F37:F40&gt;F40))+1</f>
         <v>1</v>
@@ -30085,37 +30085,37 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="88" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C88" s="194" t="str">
         <f>Matches!B49</f>
-        <v>France</v>
+        <v>Portugal</v>
       </c>
     </row>
-    <row r="89" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="89" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C89" s="194" t="str">
         <f>Matches!B50</f>
-        <v>Belgium</v>
+        <v>France</v>
       </c>
     </row>
-    <row r="90" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="90" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C90" s="194" t="str">
         <f>Matches!B51</f>
-        <v>Italy</v>
+        <v>England</v>
       </c>
     </row>
-    <row r="91" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="91" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C91" s="194" t="str">
         <f>Matches!B52</f>
-        <v>England</v>
+        <v>Belgium</v>
       </c>
     </row>
-    <row r="93" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="93" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C93" s="194" t="str">
         <f>Matches!B55</f>
         <v>France</v>
       </c>
     </row>
-    <row r="94" spans="3:3" x14ac:dyDescent="0.15">
+    <row r="94" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C94" s="194" t="str">
         <f>Matches!B56</f>
         <v>England</v>

</xml_diff>